<commit_message>
Draw timeline of raw popularity
</commit_message>
<xml_diff>
--- a/data/raw_popularity_presidents.xlsx
+++ b/data/raw_popularity_presidents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex_andorra/repos/pollsposition_models/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE336507-5ECC-CB46-B825-F1F2C250F382}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{072B3723-42CA-FA49-8355-DBB30262B723}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -478,11 +478,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1876"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1849" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A1845" workbookViewId="0">
+      <selection activeCell="J1571" sqref="J1571"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Finished formatting data for raw first GP
</commit_message>
<xml_diff>
--- a/data/raw_popularity_presidents.xlsx
+++ b/data/raw_popularity_presidents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex_andorra/repos/pollsposition_models/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{072B3723-42CA-FA49-8355-DBB30262B723}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89DC84A0-7DDB-694A-B54D-E2CA50B16E57}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -478,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1876"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1845" workbookViewId="0">
-      <selection activeCell="J1571" sqref="J1571"/>
+    <sheetView tabSelected="1" topLeftCell="A574" workbookViewId="0">
+      <selection activeCell="F593" sqref="F593"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added ribbon prior pred plots and refined priors section
</commit_message>
<xml_diff>
--- a/data/raw_popularity_presidents.xlsx
+++ b/data/raw_popularity_presidents.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex_andorra/repos/pollsposition_models/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89DC84A0-7DDB-694A-B54D-E2CA50B16E57}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{247EDD05-AAAC-6143-9FD2-3E2514CCE8A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5631" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5637" uniqueCount="29">
   <si>
     <t>president</t>
   </si>
@@ -476,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1876"/>
+  <dimension ref="A1:G1878"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A574" workbookViewId="0">
-      <selection activeCell="F593" sqref="F593"/>
+    <sheetView tabSelected="1" topLeftCell="A1857" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F1878" sqref="F1878"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -43633,6 +43633,52 @@
         <v>56</v>
       </c>
     </row>
+    <row r="1877" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1877" s="2">
+        <v>44071</v>
+      </c>
+      <c r="B1877" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1877" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1877">
+        <v>1016</v>
+      </c>
+      <c r="E1877" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1877">
+        <v>39</v>
+      </c>
+      <c r="G1877">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1878" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1878" s="2">
+        <v>44072</v>
+      </c>
+      <c r="B1878" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1878" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1878">
+        <v>1000</v>
+      </c>
+      <c r="E1878" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1878">
+        <v>35</v>
+      </c>
+      <c r="G1878">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added latest Macron polls
</commit_message>
<xml_diff>
--- a/data/raw_popularity_presidents.xlsx
+++ b/data/raw_popularity_presidents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex_andorra/repos/pollsposition_models/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{247EDD05-AAAC-6143-9FD2-3E2514CCE8A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F018CF5-26AB-A345-95AD-7C3347D3B7C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5637" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5640" uniqueCount="29">
   <si>
     <t>president</t>
   </si>
@@ -476,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1878"/>
+  <dimension ref="A1:G1879"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1857" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F1878" sqref="F1878"/>
+    <sheetView tabSelected="1" topLeftCell="A1851" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H1879" sqref="H1879"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -43679,6 +43679,29 @@
         <v>61</v>
       </c>
     </row>
+    <row r="1879" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1879" s="2">
+        <v>44083</v>
+      </c>
+      <c r="B1879" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1879" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1879">
+        <v>1001</v>
+      </c>
+      <c r="E1879" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1879">
+        <v>35</v>
+      </c>
+      <c r="G1879">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated polls with latest data
</commit_message>
<xml_diff>
--- a/data/raw_popularity_presidents.xlsx
+++ b/data/raw_popularity_presidents.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10914"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex_andorra/repos/pollsposition_models/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F018CF5-26AB-A345-95AD-7C3347D3B7C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD8C1DB-3DCD-0748-9C59-811044A70A5F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5640" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5643" uniqueCount="29">
   <si>
     <t>president</t>
   </si>
@@ -476,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1879"/>
+  <dimension ref="A1:G1880"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1851" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H1879" sqref="H1879"/>
+    <sheetView tabSelected="1" topLeftCell="A1854" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H1880" sqref="H1880"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -43702,6 +43702,29 @@
         <v>57</v>
       </c>
     </row>
+    <row r="1880" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1880" s="2">
+        <v>44100</v>
+      </c>
+      <c r="B1880" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1880" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1880">
+        <v>1000</v>
+      </c>
+      <c r="E1880" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1880">
+        <v>29</v>
+      </c>
+      <c r="G1880">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add latest popularity polls
</commit_message>
<xml_diff>
--- a/data/raw_popularity_presidents.xlsx
+++ b/data/raw_popularity_presidents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex_andorra/repos/pollsposition_models/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD8C1DB-3DCD-0748-9C59-811044A70A5F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE7E035-AF3E-F446-8B31-A115D5F01596}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5643" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5646" uniqueCount="29">
   <si>
     <t>president</t>
   </si>
@@ -476,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1880"/>
+  <dimension ref="A1:G1881"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1854" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H1880" sqref="H1880"/>
+      <selection activeCell="H1881" sqref="H1881"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -43725,6 +43725,29 @@
         <v>68</v>
       </c>
     </row>
+    <row r="1881" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1881" s="2">
+        <v>44111</v>
+      </c>
+      <c r="B1881" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1881" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1881">
+        <v>1000</v>
+      </c>
+      <c r="E1881" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1881">
+        <v>32</v>
+      </c>
+      <c r="G1881">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>